<commit_message>
CourseWork Done and Dusted!!!
</commit_message>
<xml_diff>
--- a/tournament/matches/Kolkata_England_vs_Rajastan_Australia.xlsx
+++ b/tournament/matches/Kolkata_England_vs_Rajastan_Australia.xlsx
@@ -556,7 +556,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jason Roy</t>
+          <t>David Warner</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -567,12 +567,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Pat Cummins</t>
+          <t xml:space="preserve"> Chris Jordan</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -580,23 +580,23 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>David Warner</t>
+          <t>Jason Roy</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>* NOT OUT</t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Josh Hazlewood</t>
         </is>
       </c>
       <c r="O2" t="n">
@@ -606,23 +606,23 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jos Buttler</t>
+          <t>Aaron Finch(C)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C3" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Adam Zampa</t>
+          <t xml:space="preserve"> Liam Livingstone</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -630,23 +630,23 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Aaron Finch(C)</t>
+          <t>Jos Buttler</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Chris Jordan</t>
+          <t xml:space="preserve"> Josh Hazlewood</t>
         </is>
       </c>
       <c r="O3" t="n">
@@ -656,23 +656,23 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dawid Malan</t>
+          <t>Mitchell Marsh</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Adam Zampa</t>
+          <t xml:space="preserve"> Adil Rashid</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -680,14 +680,14 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Mitchell Marsh</t>
+          <t>Dawid Malan</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -696,7 +696,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Chris Woakes</t>
+          <t xml:space="preserve"> Josh Hazlewood</t>
         </is>
       </c>
       <c r="O4" t="n">
@@ -706,23 +706,23 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jonny Bairstow</t>
+          <t>Steve Smith</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Bowled</t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Marcus Stionis</t>
+          <t xml:space="preserve"> Chris Jordan</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -730,23 +730,23 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Steve Smith</t>
+          <t>Jonny Bairstow</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="L5" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Bowled</t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mark Wood</t>
+          <t xml:space="preserve"> Mitchell Starc</t>
         </is>
       </c>
       <c r="O5" t="n">
@@ -756,23 +756,23 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Eoin Morgan(C)</t>
+          <t>Glenn Maxwell</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Bowled</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Marcus Stionis</t>
+          <t xml:space="preserve"> Chris Jordan</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -780,23 +780,23 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Glenn Maxwell</t>
+          <t>Eoin Morgan(C)</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mark Wood</t>
+          <t xml:space="preserve"> Adam Zampa</t>
         </is>
       </c>
       <c r="O6" t="n">
@@ -806,23 +806,23 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Moeen Ali</t>
+          <t>Matthew Wade</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
         <v>2</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Marcus Stionis</t>
+          <t xml:space="preserve"> Liam Livingstone</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -830,23 +830,23 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Matthew Wade</t>
+          <t>Moeen Ali</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>NOT OUT</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Mitchell Starc</t>
         </is>
       </c>
       <c r="O7" t="n">
@@ -856,14 +856,14 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Liam Livingstone</t>
+          <t>Marcus Stionis</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -872,7 +872,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Josh Hazlewood</t>
+          <t xml:space="preserve"> Chris Jordan</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -880,23 +880,23 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Marcus Stionis</t>
+          <t>Liam Livingstone</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Mitchell Starc</t>
         </is>
       </c>
       <c r="O8" t="n">
@@ -906,23 +906,23 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Chris Woakes</t>
+          <t>Pat Cummins</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Josh Hazlewood</t>
+          <t xml:space="preserve"> Adil Rashid</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -930,23 +930,23 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Pat Cummins</t>
+          <t>Chris Woakes</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Marcus Stionis</t>
         </is>
       </c>
       <c r="O9" t="n">
@@ -956,14 +956,14 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Chris Jordan</t>
+          <t>Mitchell Starc</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -972,7 +972,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Josh Hazlewood</t>
+          <t xml:space="preserve"> Liam Livingstone</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -980,18 +980,18 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Mitchell Starc</t>
+          <t>Chris Jordan</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>NOT OUT</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1006,23 +1006,23 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Adil Rashid</t>
+          <t>Adam Zampa</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>NOT OUT</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Chris Jordan</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -1030,23 +1030,23 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Adam Zampa</t>
+          <t>Adil Rashid</t>
         </is>
       </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Mitchell Starc</t>
         </is>
       </c>
       <c r="O11" t="n">
@@ -1056,23 +1056,23 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Mark Wood</t>
+          <t>Josh Hazlewood</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>NOT OUT</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Pat Cummins</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -1080,23 +1080,23 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Josh Hazlewood</t>
+          <t>Mark Wood</t>
         </is>
       </c>
       <c r="K12" t="n">
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Mitchell Starc</t>
         </is>
       </c>
       <c r="O12" t="n">
@@ -1147,32 +1147,32 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>111</v>
+        <v>191</v>
       </c>
       <c r="B16" t="n">
         <v>10</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>14.1</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="J16" t="n">
         <v>114</v>
       </c>
       <c r="K16" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20">
@@ -1230,66 +1230,66 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Marcus Stionis</t>
+          <t>Mark Wood</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>44</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>14.67</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Pat Cummins</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="C21" t="n">
-        <v>4</v>
-      </c>
-      <c r="D21" t="n">
-        <v>3</v>
-      </c>
-      <c r="E21" t="n">
-        <v>4</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Chris Jordan</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
       <c r="L21" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="M21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Josh Hazlewood</t>
+          <t>Adil Rashid</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" t="n">
-        <v>14.5</v>
+        <v>13.33</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Chris Woakes</t>
+          <t>Marcus Stionis</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1298,78 +1298,78 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="M22" t="n">
         <v>1</v>
       </c>
       <c r="N22" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Adam Zampa</t>
+          <t>Chris Jordan</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>30</v>
+      </c>
+      <c r="D23" t="n">
+        <v>5</v>
+      </c>
+      <c r="E23" t="n">
+        <v>10</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Josh Hazlewood</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
           <t>2.0</t>
         </is>
       </c>
-      <c r="C23" t="n">
-        <v>32</v>
-      </c>
-      <c r="D23" t="n">
-        <v>2</v>
-      </c>
-      <c r="E23" t="n">
-        <v>16</v>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>Liam Livingstone</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
       <c r="L23" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N23" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Mitchell Starc</t>
+          <t>Chris Woakes</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>15.5</v>
+        <v>19.33</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Mark Wood</t>
+          <t>Adam Zampa</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -1378,66 +1378,66 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="M24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N24" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Pat Cummins</t>
+          <t>Liam Livingstone</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1.3</t>
+          <t>2.1</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25" t="n">
-        <v>11.54</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Adil Rashid</t>
+          <t>Mitchell Starc</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="M25" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N25" t="n">
-        <v>20.83</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
       <c r="F27" t="inlineStr">
         <is>
-          <t>Rajastan Australia Won the toss and chose to bowl</t>
+          <t>Rajastan Australia Won the toss and chose to bat</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="F28" t="inlineStr">
         <is>
-          <t>Rajastan Australia Won by 6 wickets</t>
+          <t>Rajastan Australia Won by 77 runs</t>
         </is>
       </c>
     </row>

</xml_diff>